<commit_message>
Update environment for 5G
</commit_message>
<xml_diff>
--- a/config/prod/RawFilePathCollection.xlsx
+++ b/config/prod/RawFilePathCollection.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Granite\New Equipment\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Libraries\git\true\RanBaselineApp\source\config\prod\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8FC101B-F0D2-4D96-ADC6-FD6D7181DB5C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46785452-BB43-45C6-9DA6-374EAD49CD21}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{F32754BE-CF86-49F4-BEFD-53C8D448A04A}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{F32754BE-CF86-49F4-BEFD-53C8D448A04A}"/>
   </bookViews>
   <sheets>
     <sheet name="Path" sheetId="2" r:id="rId1"/>
@@ -21,9 +21,9 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Backup!$A$1:$I$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Backup (2)'!$A$1:$I$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Path!$A$1:$I$62</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Path!$A$1:$I$65</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +31,10 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -44,7 +47,7 @@
     <author>my</author>
   </authors>
   <commentList>
-    <comment ref="G50" authorId="0" shapeId="0" xr:uid="{5D21C560-AADE-704C-A077-71D2B57234F2}">
+    <comment ref="G53" authorId="0" shapeId="0" xr:uid="{5D21C560-AADE-704C-A077-71D2B57234F2}">
       <text>
         <r>
           <rPr>
@@ -201,7 +204,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1480" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1504" uniqueCount="170">
   <si>
     <t>ZTE</t>
   </si>
@@ -699,6 +702,18 @@
   </si>
   <si>
     <t>/home/app/ngoss/data/rfserver/Ericsson/NTH-ENM/full_kget/MIXEDMODE_LW/1Current</t>
+  </si>
+  <si>
+    <t>NR</t>
+  </si>
+  <si>
+    <t>/home/app/ngoss/data/rfserver/Ericsson/NTH-ENM/full_kget/RADIONODE_NR/1Current/</t>
+  </si>
+  <si>
+    <t>/home/app/ngoss/data/rfserver/Ericsson/CEW-ENM/full_kget/RADIONODE_NR/1Current/</t>
+  </si>
+  <si>
+    <t>/home/app/ngoss/data/rfserver/Ericsson/STH-ENM/full_kget/RADIONODE_NR/1Current/</t>
   </si>
 </sst>
 </file>
@@ -1233,26 +1248,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B114B3C2-9B56-4F69-A484-BA4ED1CFE527}">
-  <dimension ref="A1:I62"/>
+  <dimension ref="A1:I65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D57" sqref="D57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.19921875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="13.6640625" style="24" customWidth="1"/>
     <col min="2" max="2" width="13.6640625" style="26" customWidth="1"/>
-    <col min="3" max="3" width="15.44140625" style="26" customWidth="1"/>
-    <col min="4" max="4" width="15.21875" style="24" customWidth="1"/>
+    <col min="3" max="3" width="15.46484375" style="26" customWidth="1"/>
+    <col min="4" max="4" width="15.19921875" style="24" customWidth="1"/>
     <col min="5" max="6" width="13.6640625" style="24" customWidth="1"/>
-    <col min="7" max="7" width="107.21875" style="26" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="107.19921875" style="26" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="46" style="26" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="29.21875" style="24" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.21875" style="24"/>
+    <col min="9" max="9" width="29.19921875" style="24" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.19921875" style="24"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="28" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" s="28" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="29" t="s">
         <v>2</v>
       </c>
@@ -1281,7 +1296,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A2" s="23" t="s">
         <v>8</v>
       </c>
@@ -1310,7 +1325,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A3" s="23" t="s">
         <v>8</v>
       </c>
@@ -1339,7 +1354,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A4" s="23" t="s">
         <v>8</v>
       </c>
@@ -1368,7 +1383,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A5" s="23" t="s">
         <v>8</v>
       </c>
@@ -1397,7 +1412,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A6" s="23" t="s">
         <v>8</v>
       </c>
@@ -1426,7 +1441,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A7" s="23" t="s">
         <v>8</v>
       </c>
@@ -1455,7 +1470,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="8" spans="1:9" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" s="31" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A8" s="23" t="s">
         <v>8</v>
       </c>
@@ -1484,7 +1499,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A9" s="23" t="s">
         <v>8</v>
       </c>
@@ -1513,7 +1528,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A10" s="23" t="s">
         <v>8</v>
       </c>
@@ -1542,7 +1557,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A11" s="23" t="s">
         <v>8</v>
       </c>
@@ -1571,7 +1586,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A12" s="23" t="s">
         <v>8</v>
       </c>
@@ -1600,7 +1615,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A13" s="23" t="s">
         <v>8</v>
       </c>
@@ -1629,7 +1644,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A14" s="23" t="s">
         <v>8</v>
       </c>
@@ -1658,7 +1673,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A15" s="23" t="s">
         <v>8</v>
       </c>
@@ -1687,7 +1702,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A16" s="23" t="s">
         <v>8</v>
       </c>
@@ -1716,7 +1731,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A17" s="23" t="s">
         <v>8</v>
       </c>
@@ -1745,7 +1760,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A18" s="23" t="s">
         <v>8</v>
       </c>
@@ -1774,7 +1789,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A19" s="23" t="s">
         <v>8</v>
       </c>
@@ -1803,7 +1818,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A20" s="23" t="s">
         <v>8</v>
       </c>
@@ -1832,7 +1847,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A21" s="23" t="s">
         <v>8</v>
       </c>
@@ -1861,7 +1876,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A22" s="23" t="s">
         <v>8</v>
       </c>
@@ -1890,7 +1905,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A23" s="23" t="s">
         <v>8</v>
       </c>
@@ -1919,7 +1934,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A24" s="23" t="s">
         <v>8</v>
       </c>
@@ -1948,7 +1963,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A25" s="23" t="s">
         <v>8</v>
       </c>
@@ -1977,7 +1992,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A26" s="23" t="s">
         <v>8</v>
       </c>
@@ -2006,7 +2021,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A27" s="23" t="s">
         <v>8</v>
       </c>
@@ -2035,7 +2050,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A28" s="23" t="s">
         <v>8</v>
       </c>
@@ -2064,7 +2079,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A29" s="23" t="s">
         <v>8</v>
       </c>
@@ -2093,7 +2108,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A30" s="23" t="s">
         <v>8</v>
       </c>
@@ -2122,7 +2137,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A31" s="23" t="s">
         <v>8</v>
       </c>
@@ -2151,7 +2166,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A32" s="23" t="s">
         <v>8</v>
       </c>
@@ -2180,7 +2195,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A33" s="23" t="s">
         <v>8</v>
       </c>
@@ -2209,7 +2224,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A34" s="23" t="s">
         <v>8</v>
       </c>
@@ -2238,7 +2253,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A35" s="23" t="s">
         <v>8</v>
       </c>
@@ -2267,7 +2282,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A36" s="23" t="s">
         <v>8</v>
       </c>
@@ -2296,7 +2311,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A37" s="23" t="s">
         <v>8</v>
       </c>
@@ -2325,7 +2340,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A38" s="23" t="s">
         <v>8</v>
       </c>
@@ -2354,7 +2369,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A39" s="23" t="s">
         <v>8</v>
       </c>
@@ -2383,7 +2398,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A40" s="23" t="s">
         <v>8</v>
       </c>
@@ -2412,7 +2427,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A41" s="23" t="s">
         <v>8</v>
       </c>
@@ -2441,7 +2456,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A42" s="23" t="s">
         <v>8</v>
       </c>
@@ -2470,7 +2485,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A43" s="23" t="s">
         <v>8</v>
       </c>
@@ -2499,7 +2514,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A44" s="23" t="s">
         <v>8</v>
       </c>
@@ -2528,94 +2543,94 @@
         <v>52</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A45" s="23" t="s">
         <v>8</v>
       </c>
       <c r="B45" s="25" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="C45" s="25" t="s">
-        <v>11</v>
+        <v>166</v>
       </c>
       <c r="D45" s="23">
-        <v>900</v>
+        <v>2600</v>
       </c>
       <c r="E45" s="23" t="s">
-        <v>34</v>
+        <v>55</v>
       </c>
       <c r="F45" s="23" t="s">
         <v>13</v>
       </c>
       <c r="G45" s="25" t="s">
-        <v>63</v>
+        <v>167</v>
       </c>
       <c r="H45" s="25" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="I45" s="23" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A46" s="23" t="s">
         <v>8</v>
       </c>
       <c r="B46" s="25" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="C46" s="25" t="s">
-        <v>11</v>
+        <v>166</v>
       </c>
       <c r="D46" s="23">
-        <v>900</v>
+        <v>2600</v>
       </c>
       <c r="E46" s="23" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="F46" s="23" t="s">
         <v>13</v>
       </c>
       <c r="G46" s="25" t="s">
-        <v>64</v>
+        <v>168</v>
       </c>
       <c r="H46" s="25" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="I46" s="23" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A47" s="23" t="s">
         <v>8</v>
       </c>
       <c r="B47" s="25" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="C47" s="25" t="s">
-        <v>11</v>
+        <v>166</v>
       </c>
       <c r="D47" s="23">
-        <v>900</v>
+        <v>2600</v>
       </c>
       <c r="E47" s="23" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="F47" s="23" t="s">
         <v>13</v>
       </c>
       <c r="G47" s="25" t="s">
-        <v>65</v>
+        <v>169</v>
       </c>
       <c r="H47" s="25" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="I47" s="23" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A48" s="23" t="s">
         <v>8</v>
       </c>
@@ -2623,10 +2638,10 @@
         <v>9</v>
       </c>
       <c r="C48" s="25" t="s">
-        <v>16</v>
-      </c>
-      <c r="D48" s="23" t="s">
-        <v>33</v>
+        <v>11</v>
+      </c>
+      <c r="D48" s="23">
+        <v>900</v>
       </c>
       <c r="E48" s="23" t="s">
         <v>34</v>
@@ -2635,16 +2650,16 @@
         <v>13</v>
       </c>
       <c r="G48" s="25" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="H48" s="25" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="I48" s="23" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A49" s="23" t="s">
         <v>8</v>
       </c>
@@ -2652,28 +2667,28 @@
         <v>9</v>
       </c>
       <c r="C49" s="25" t="s">
-        <v>16</v>
-      </c>
-      <c r="D49" s="23" t="s">
-        <v>33</v>
+        <v>11</v>
+      </c>
+      <c r="D49" s="23">
+        <v>900</v>
       </c>
       <c r="E49" s="23" t="s">
-        <v>34</v>
+        <v>57</v>
       </c>
       <c r="F49" s="23" t="s">
         <v>13</v>
       </c>
       <c r="G49" s="25" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="H49" s="25" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="I49" s="23" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A50" s="23" t="s">
         <v>8</v>
       </c>
@@ -2681,28 +2696,28 @@
         <v>9</v>
       </c>
       <c r="C50" s="25" t="s">
-        <v>16</v>
-      </c>
-      <c r="D50" s="23" t="s">
-        <v>33</v>
+        <v>11</v>
+      </c>
+      <c r="D50" s="23">
+        <v>900</v>
       </c>
       <c r="E50" s="23" t="s">
-        <v>34</v>
+        <v>58</v>
       </c>
       <c r="F50" s="23" t="s">
         <v>13</v>
       </c>
       <c r="G50" s="25" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="H50" s="25" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="I50" s="23" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A51" s="23" t="s">
         <v>8</v>
       </c>
@@ -2716,13 +2731,13 @@
         <v>33</v>
       </c>
       <c r="E51" s="23" t="s">
-        <v>57</v>
+        <v>34</v>
       </c>
       <c r="F51" s="23" t="s">
         <v>13</v>
       </c>
       <c r="G51" s="25" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="H51" s="25" t="s">
         <v>39</v>
@@ -2731,7 +2746,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A52" s="23" t="s">
         <v>8</v>
       </c>
@@ -2745,13 +2760,13 @@
         <v>33</v>
       </c>
       <c r="E52" s="23" t="s">
-        <v>58</v>
+        <v>34</v>
       </c>
       <c r="F52" s="23" t="s">
         <v>13</v>
       </c>
       <c r="G52" s="25" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="H52" s="25" t="s">
         <v>39</v>
@@ -2760,18 +2775,18 @@
         <v>40</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A53" s="23" t="s">
-        <v>37</v>
+        <v>8</v>
       </c>
       <c r="B53" s="25" t="s">
         <v>9</v>
       </c>
       <c r="C53" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="D53" s="23">
-        <v>850</v>
+        <v>16</v>
+      </c>
+      <c r="D53" s="23" t="s">
+        <v>33</v>
       </c>
       <c r="E53" s="23" t="s">
         <v>34</v>
@@ -2780,45 +2795,45 @@
         <v>13</v>
       </c>
       <c r="G53" s="25" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="H53" s="25" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="I53" s="23" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A54" s="23" t="s">
-        <v>37</v>
+        <v>8</v>
       </c>
       <c r="B54" s="25" t="s">
         <v>9</v>
       </c>
       <c r="C54" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="D54" s="23">
-        <v>850</v>
+        <v>16</v>
+      </c>
+      <c r="D54" s="23" t="s">
+        <v>33</v>
       </c>
       <c r="E54" s="23" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F54" s="23" t="s">
         <v>13</v>
       </c>
       <c r="G54" s="25" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="H54" s="25" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="I54" s="23" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A55" s="23" t="s">
         <v>8</v>
       </c>
@@ -2826,30 +2841,30 @@
         <v>9</v>
       </c>
       <c r="C55" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="D55" s="23">
-        <v>2100</v>
+        <v>16</v>
+      </c>
+      <c r="D55" s="23" t="s">
+        <v>33</v>
       </c>
       <c r="E55" s="23" t="s">
-        <v>34</v>
+        <v>58</v>
       </c>
       <c r="F55" s="23" t="s">
         <v>13</v>
       </c>
       <c r="G55" s="25" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
       <c r="H55" s="25" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="I55" s="23" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A56" s="23" t="s">
-        <v>8</v>
+        <v>37</v>
       </c>
       <c r="B56" s="25" t="s">
         <v>9</v>
@@ -2858,16 +2873,16 @@
         <v>1</v>
       </c>
       <c r="D56" s="23">
-        <v>2100</v>
+        <v>850</v>
       </c>
       <c r="E56" s="23" t="s">
-        <v>57</v>
+        <v>34</v>
       </c>
       <c r="F56" s="23" t="s">
         <v>13</v>
       </c>
       <c r="G56" s="25" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="H56" s="25" t="s">
         <v>35</v>
@@ -2876,9 +2891,9 @@
         <v>38</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A57" s="23" t="s">
-        <v>8</v>
+        <v>37</v>
       </c>
       <c r="B57" s="25" t="s">
         <v>9</v>
@@ -2887,16 +2902,16 @@
         <v>1</v>
       </c>
       <c r="D57" s="23">
-        <v>2100</v>
+        <v>850</v>
       </c>
       <c r="E57" s="23" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="F57" s="23" t="s">
         <v>13</v>
       </c>
       <c r="G57" s="25" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="H57" s="25" t="s">
         <v>35</v>
@@ -2905,115 +2920,121 @@
         <v>38</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A58" s="23" t="s">
         <v>8</v>
       </c>
       <c r="B58" s="25" t="s">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="C58" s="25" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="D58" s="23">
-        <v>900</v>
-      </c>
-      <c r="E58" s="23"/>
+        <v>2100</v>
+      </c>
+      <c r="E58" s="23" t="s">
+        <v>34</v>
+      </c>
       <c r="F58" s="23" t="s">
         <v>13</v>
       </c>
       <c r="G58" s="25" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="H58" s="25" t="s">
-        <v>159</v>
+        <v>35</v>
       </c>
       <c r="I58" s="23" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A59" s="23" t="s">
         <v>8</v>
       </c>
       <c r="B59" s="25" t="s">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="C59" s="25" t="s">
-        <v>16</v>
-      </c>
-      <c r="D59" s="23" t="s">
-        <v>33</v>
-      </c>
-      <c r="E59" s="23"/>
+        <v>1</v>
+      </c>
+      <c r="D59" s="23">
+        <v>2100</v>
+      </c>
+      <c r="E59" s="23" t="s">
+        <v>57</v>
+      </c>
       <c r="F59" s="23" t="s">
         <v>13</v>
       </c>
       <c r="G59" s="25" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="H59" s="25" t="s">
-        <v>160</v>
-      </c>
-      <c r="I59" s="23"/>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
+        <v>35</v>
+      </c>
+      <c r="I59" s="23" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A60" s="23" t="s">
-        <v>37</v>
+        <v>8</v>
       </c>
       <c r="B60" s="25" t="s">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="C60" s="25" t="s">
         <v>1</v>
       </c>
       <c r="D60" s="23">
-        <v>850</v>
+        <v>2100</v>
       </c>
       <c r="E60" s="23" t="s">
-        <v>43</v>
+        <v>58</v>
       </c>
       <c r="F60" s="23" t="s">
         <v>13</v>
       </c>
       <c r="G60" s="25" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="H60" s="25" t="s">
-        <v>161</v>
+        <v>35</v>
       </c>
       <c r="I60" s="23" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A61" s="23" t="s">
-        <v>37</v>
+        <v>8</v>
       </c>
       <c r="B61" s="25" t="s">
         <v>0</v>
       </c>
       <c r="C61" s="25" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="D61" s="23">
-        <v>850</v>
+        <v>900</v>
       </c>
       <c r="E61" s="23"/>
       <c r="F61" s="23" t="s">
         <v>13</v>
       </c>
       <c r="G61" s="25" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="H61" s="25" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="I61" s="23" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A62" s="23" t="s">
         <v>8</v>
       </c>
@@ -3021,24 +3042,105 @@
         <v>0</v>
       </c>
       <c r="C62" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="D62" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="E62" s="23"/>
+      <c r="F62" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="G62" s="25" t="s">
+        <v>79</v>
+      </c>
+      <c r="H62" s="25" t="s">
+        <v>160</v>
+      </c>
+      <c r="I62" s="23"/>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A63" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="B63" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="C63" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="D62" s="23">
+      <c r="D63" s="23">
+        <v>850</v>
+      </c>
+      <c r="E63" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="F63" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="G63" s="25" t="s">
+        <v>77</v>
+      </c>
+      <c r="H63" s="25" t="s">
+        <v>161</v>
+      </c>
+      <c r="I63" s="23" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A64" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="B64" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="C64" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="D64" s="23">
+        <v>850</v>
+      </c>
+      <c r="E64" s="23"/>
+      <c r="F64" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="G64" s="25" t="s">
+        <v>78</v>
+      </c>
+      <c r="H64" s="25" t="s">
+        <v>161</v>
+      </c>
+      <c r="I64" s="23" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A65" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="B65" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="C65" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="D65" s="23">
         <v>2100</v>
       </c>
-      <c r="E62" s="23" t="s">
+      <c r="E65" s="23" t="s">
         <v>46</v>
       </c>
-      <c r="F62" s="23" t="s">
-        <v>13</v>
-      </c>
-      <c r="G62" s="25" t="s">
+      <c r="F65" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="G65" s="25" t="s">
         <v>80</v>
       </c>
-      <c r="H62" s="25" t="s">
+      <c r="H65" s="25" t="s">
         <v>161</v>
       </c>
-      <c r="I62" s="23" t="s">
+      <c r="I65" s="23" t="s">
         <v>45</v>
       </c>
     </row>
@@ -3057,30 +3159,30 @@
       <selection activeCell="A2" sqref="A2:I31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="7.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.796875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.46484375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="104.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="104.46484375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="38" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="25.44140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="70.77734375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25.46484375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="70.796875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="65.6640625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="65.6640625" customWidth="1"/>
     <col min="15" max="15" width="76.6640625" customWidth="1"/>
-    <col min="16" max="16" width="9.21875" customWidth="1"/>
-    <col min="17" max="17" width="11.44140625" customWidth="1"/>
-    <col min="18" max="18" width="10.44140625" customWidth="1"/>
+    <col min="16" max="16" width="9.19921875" customWidth="1"/>
+    <col min="17" max="17" width="11.46484375" customWidth="1"/>
+    <col min="18" max="18" width="10.46484375" customWidth="1"/>
     <col min="19" max="19" width="65" customWidth="1"/>
-    <col min="20" max="20" width="70.77734375" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="39.44140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="70.796875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="39.46484375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
@@ -3109,7 +3211,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A2" s="7" t="s">
         <v>8</v>
       </c>
@@ -3168,7 +3270,7 @@
         <v>rfserver_clone/Ericsson/CEW/CNA_FULL/1Current</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A3" s="7" t="s">
         <v>8</v>
       </c>
@@ -3223,7 +3325,7 @@
         <v>rfserver_clone/Ericsson/CEW/EXERT/1Current/</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A4" s="7" t="s">
         <v>8</v>
       </c>
@@ -3278,7 +3380,7 @@
         <v>rfserver_clone/Ericsson/NTH/CNA_FULL/1Current/</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A5" s="7" t="s">
         <v>8</v>
       </c>
@@ -3333,7 +3435,7 @@
         <v>rfserver_clone/Ericsson/NTH/EXERT/1Current/</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A6" s="7" t="s">
         <v>8</v>
       </c>
@@ -3388,7 +3490,7 @@
         <v>rfserver_clone/Ericsson/STH/CNA_FULL/1Current/</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A7" s="7" t="s">
         <v>8</v>
       </c>
@@ -3443,7 +3545,7 @@
         <v>rfserver_clone/Ericsson/STH/EXERT/1Current/</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A8" s="7" t="s">
         <v>8</v>
       </c>
@@ -3498,7 +3600,7 @@
         <v>rfserver_clone/Ericsson/CEW/full_kget/ENB/1Current/</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A9" s="7" t="s">
         <v>8</v>
       </c>
@@ -3553,7 +3655,7 @@
         <v>rfserver_clone/Ericsson/CEW/full_kget/RADIONODE/1Current/</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A10" s="7" t="s">
         <v>8</v>
       </c>
@@ -3608,7 +3710,7 @@
         <v>rfserver_clone/Ericsson/CEW/full_kget/MIXEDMODE_LW/1Current/</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A11" s="7" t="s">
         <v>8</v>
       </c>
@@ -3663,7 +3765,7 @@
         <v>rfserver_clone/Ericsson/CEW/full_kget/MIXEDMODE_LG/1Current/</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A12" s="7" t="s">
         <v>8</v>
       </c>
@@ -3718,7 +3820,7 @@
         <v>rfserver_clone/Ericsson/NTH-ENM/full_kget/ENB/1Current/</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A13" s="7" t="s">
         <v>8</v>
       </c>
@@ -3773,7 +3875,7 @@
         <v>rfserver_clone/Ericsson/NTH-ENM/full_kget/RADIONODE/1Current/</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A14" s="7" t="s">
         <v>8</v>
       </c>
@@ -3828,7 +3930,7 @@
         <v>rfserver_clone/Ericsson/NTH/full_kget/MIXEDMODE_LW/1Current/</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A15" s="7" t="s">
         <v>8</v>
       </c>
@@ -3883,7 +3985,7 @@
         <v>rfserver_clone/Ericsson/NTH/full_kget/MIXEDMODE_LG/1Current/</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A16" s="7" t="s">
         <v>8</v>
       </c>
@@ -3938,7 +4040,7 @@
         <v>rfserver_clone/Ericsson/STH/full_kget/ENB/1Current/</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A17" s="7" t="s">
         <v>8</v>
       </c>
@@ -3993,7 +4095,7 @@
         <v>rfserver_clone/Ericsson/STH/full_kget/RADIONODE/1Current/</v>
       </c>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A18" s="7" t="s">
         <v>8</v>
       </c>
@@ -4048,7 +4150,7 @@
         <v>rfserver_clone/Ericsson/STH/full_kget/MIXEDMODE_LW/1Current/</v>
       </c>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A19" s="7" t="s">
         <v>8</v>
       </c>
@@ -4103,7 +4205,7 @@
         <v>rfserver_clone/Ericsson/STH/full_kget/MIXEDMODE_LG/1Current/</v>
       </c>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A20" s="7" t="s">
         <v>8</v>
       </c>
@@ -4158,7 +4260,7 @@
         <v>rfserver_clone/Ericsson/CEW/full_kget/RNC/1Current/</v>
       </c>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A21" s="7" t="s">
         <v>8</v>
       </c>
@@ -4213,7 +4315,7 @@
         <v>rfserver_clone/Ericsson/CEW/full_kget/RBS/1Current/</v>
       </c>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A22" s="7" t="s">
         <v>8</v>
       </c>
@@ -4268,7 +4370,7 @@
         <v>rfserver_clone/Ericsson/CEW/full_kget/RADIONODE_WCDMA/1Current/</v>
       </c>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A23" s="7" t="s">
         <v>8</v>
       </c>
@@ -4323,7 +4425,7 @@
         <v>rfserver_clone/Ericsson/CEW/full_kget/MIXEDMODE_WG/1Current/</v>
       </c>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A24" s="7" t="s">
         <v>8</v>
       </c>
@@ -4378,7 +4480,7 @@
         <v>rfserver_clone/Ericsson/NTH/full_kget/RNC/1Current/</v>
       </c>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A25" s="7" t="s">
         <v>8</v>
       </c>
@@ -4433,7 +4535,7 @@
         <v>rfserver_clone/Ericsson/NTH/full_kget/RBS/1Current/</v>
       </c>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A26" s="7" t="s">
         <v>8</v>
       </c>
@@ -4488,7 +4590,7 @@
         <v>rfserver_clone/Ericsson/NTH/full_kget/RADIONODE_WCDMA/1Current/</v>
       </c>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A27" s="7" t="s">
         <v>8</v>
       </c>
@@ -4543,7 +4645,7 @@
         <v>rfserver_clone/Ericsson/NTH/full_kget/MIXEDMODE_WG/1Current/</v>
       </c>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A28" s="7" t="s">
         <v>8</v>
       </c>
@@ -4598,7 +4700,7 @@
         <v>rfserver_clone/Ericsson/STH/full_kget/RNC/1Current/</v>
       </c>
     </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A29" s="7" t="s">
         <v>8</v>
       </c>
@@ -4653,7 +4755,7 @@
         <v>rfserver_clone/Ericsson/STH/full_kget/RBS/1Current/</v>
       </c>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A30" s="7" t="s">
         <v>8</v>
       </c>
@@ -4708,7 +4810,7 @@
         <v>rfserver_clone/Ericsson/STH/full_kget/RADIONODE_WCDMA/1Current/</v>
       </c>
     </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A31" s="7" t="s">
         <v>8</v>
       </c>
@@ -4763,7 +4865,7 @@
         <v>rfserver_clone/Ericsson/STH/full_kget/MIXEDMODE_WG/1Current/</v>
       </c>
     </row>
-    <row r="32" spans="1:20" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:20" s="17" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A32" s="15" t="s">
         <v>8</v>
       </c>
@@ -4821,7 +4923,7 @@
         <v>rfserver_clone/Huawei2100/BMA/BSC_CFGMML/1Current/unzip-ngoss-drop2-expansion/</v>
       </c>
     </row>
-    <row r="33" spans="1:20" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:20" s="17" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A33" s="15" t="s">
         <v>8</v>
       </c>
@@ -4879,7 +4981,7 @@
         <v>rfserver_clone/Huawei2100/EAS/BSC_CFGMML/1Current/unzip-ngoss-drop2-expansion/</v>
       </c>
     </row>
-    <row r="34" spans="1:20" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:20" s="17" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A34" s="15" t="s">
         <v>8</v>
       </c>
@@ -4937,7 +5039,7 @@
         <v>rfserver_clone/Huawei2100/NOE/BSC_CFGMML/1Current/unzip-ngoss-drop2-expansion/</v>
       </c>
     </row>
-    <row r="35" spans="1:20" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:20" s="17" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A35" s="20" t="s">
         <v>8</v>
       </c>
@@ -4995,7 +5097,7 @@
         <v>rfserver_clone/UtranLTE/BMA/BTS3900_LTE/1Current/unzip-ngoss-drop2-expansion/</v>
       </c>
     </row>
-    <row r="36" spans="1:20" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:20" s="17" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A36" s="20" t="s">
         <v>8</v>
       </c>
@@ -5053,7 +5155,7 @@
         <v>rfserver_clone/UtranLTE/BMA/BTS3900_LTE2/1Current/unzip-ngoss-drop2-expansion/</v>
       </c>
     </row>
-    <row r="37" spans="1:20" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:20" s="17" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A37" s="21" t="s">
         <v>8</v>
       </c>
@@ -5111,7 +5213,7 @@
         <v>rfserver_clone/UtranLTE/BMA/BTS3900_LTE3/1Current/unzip-ngoss-drop2-expansion/</v>
       </c>
     </row>
-    <row r="38" spans="1:20" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:20" s="17" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A38" s="20" t="s">
         <v>8</v>
       </c>
@@ -5169,7 +5271,7 @@
         <v>rfserver_clone/UtranLTE/EAS/BTS3900_LTE/1Current/unzip-ngoss-drop2-expansion/</v>
       </c>
     </row>
-    <row r="39" spans="1:20" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:20" s="17" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A39" s="22" t="s">
         <v>8</v>
       </c>
@@ -5227,7 +5329,7 @@
         <v>rfserver_clone/UtranLTE/NOE/BTS3900_LTE/1Current/unzip-ngoss-drop2-expansion/</v>
       </c>
     </row>
-    <row r="40" spans="1:20" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:20" s="17" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A40" s="15" t="s">
         <v>37</v>
       </c>
@@ -5285,7 +5387,7 @@
         <v>rfserver_clone/Huawei/BMA/CFGMML/1Current/unzip-ngoss-drop2-expansion/</v>
       </c>
     </row>
-    <row r="41" spans="1:20" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:20" s="17" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A41" s="15" t="s">
         <v>37</v>
       </c>
@@ -5343,7 +5445,7 @@
         <v>rfserver_clone/Huawei/UPC/CFGMML/1Current/unzip-ngoss-drop2-expansion/</v>
       </c>
     </row>
-    <row r="42" spans="1:20" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:20" s="17" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A42" s="15" t="s">
         <v>8</v>
       </c>
@@ -5401,7 +5503,7 @@
         <v>rfserver_clone/Huawei2100/BMA/CFGMML/1Current/unzip-ngoss-drop2-expansion/</v>
       </c>
     </row>
-    <row r="43" spans="1:20" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:20" s="17" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A43" s="15" t="s">
         <v>8</v>
       </c>
@@ -5459,7 +5561,7 @@
         <v>rfserver_clone/Huawei2100/EAS/CFGMML/1Current/unzip-ngoss-drop2-expansion/</v>
       </c>
     </row>
-    <row r="44" spans="1:20" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:20" s="17" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A44" s="15" t="s">
         <v>8</v>
       </c>
@@ -5517,7 +5619,7 @@
         <v>rfserver_clone/Huawei2100/NOE/CFGMML/1Current/unzip-ngoss-drop2-expansion/</v>
       </c>
     </row>
-    <row r="45" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A45" s="9" t="s">
         <v>8</v>
       </c>
@@ -5570,7 +5672,7 @@
         <v>rfserver_clone/ZTE2100/radio/1Current/unzip-ngoss-drop2-expansion/</v>
       </c>
     </row>
-    <row r="46" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A46" s="7" t="s">
         <v>8</v>
       </c>
@@ -5621,7 +5723,7 @@
         <v>rfserver_clone/ZTE2100/bulkcm/1Current/unzip-ngoss-drop2-expansion/</v>
       </c>
     </row>
-    <row r="47" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A47" s="8" t="s">
         <v>37</v>
       </c>
@@ -5676,7 +5778,7 @@
         <v>rfserver_clone/ZTE/radio_CW/1Current/unzip-ngoss-drop2-expansion/</v>
       </c>
     </row>
-    <row r="48" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A48" s="8" t="s">
         <v>37</v>
       </c>
@@ -5729,7 +5831,7 @@
         <v>rfserver_clone/ZTE/radio_STH/1Current/unzip-ngoss-drop2-expansion/</v>
       </c>
     </row>
-    <row r="49" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A49" s="9" t="s">
         <v>8</v>
       </c>
@@ -5784,7 +5886,7 @@
         <v>rfserver_clone/ZTE2100/equip/1Current/unzip-ngoss-drop2-expansion/</v>
       </c>
     </row>
-    <row r="50" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
@@ -5805,31 +5907,31 @@
         <v/>
       </c>
     </row>
-    <row r="51" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:20" x14ac:dyDescent="0.45">
       <c r="T51" s="10" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="52" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:20" x14ac:dyDescent="0.45">
       <c r="T52" s="10" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="53" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:20" x14ac:dyDescent="0.45">
       <c r="T53" s="10" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="54" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:20" x14ac:dyDescent="0.45">
       <c r="T54" s="10" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="55" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:20" x14ac:dyDescent="0.45">
       <c r="T55" s="10" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -5851,20 +5953,20 @@
       <selection activeCell="I13" activeCellId="1" sqref="B5 I13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.46484375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.77734375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="35.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.44140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="21.77734375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="20.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.46484375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.796875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="35.46484375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.46484375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21.796875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.46484375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A1" s="4" t="s">
         <v>6</v>
       </c>
@@ -5896,7 +5998,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A2" s="32" t="s">
         <v>9</v>
       </c>
@@ -5920,7 +6022,7 @@
       </c>
       <c r="K2" s="2"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A3" s="32"/>
       <c r="B3" s="1" t="s">
         <v>20</v>
@@ -5942,7 +6044,7 @@
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A4" s="32"/>
       <c r="B4" s="1" t="s">
         <v>21</v>
@@ -5960,7 +6062,7 @@
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A5" s="32"/>
       <c r="B5" s="1" t="s">
         <v>22</v>
@@ -5983,7 +6085,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A6" s="32" t="s">
         <v>0</v>
       </c>
@@ -6007,7 +6109,7 @@
       </c>
       <c r="K6" s="2"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A7" s="32"/>
       <c r="B7" s="1" t="s">
         <v>20</v>
@@ -6031,7 +6133,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A8" s="32"/>
       <c r="B8" s="1" t="s">
         <v>21</v>
@@ -6049,7 +6151,7 @@
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A9" s="32"/>
       <c r="B9" s="1" t="s">
         <v>22</v>
@@ -6069,7 +6171,7 @@
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A10" s="32" t="s">
         <v>17</v>
       </c>
@@ -6089,7 +6191,7 @@
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A11" s="32"/>
       <c r="B11" s="1" t="s">
         <v>20</v>
@@ -6113,7 +6215,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A12" s="32"/>
       <c r="B12" s="1" t="s">
         <v>21</v>
@@ -6131,7 +6233,7 @@
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A13" s="32"/>
       <c r="B13" s="1" t="s">
         <v>22</v>
@@ -6153,7 +6255,7 @@
       </c>
       <c r="K13" s="2"/>
     </row>
-    <row r="26" spans="12:12" x14ac:dyDescent="0.3">
+    <row r="26" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L26" t="s">
         <v>23</v>
       </c>
@@ -6179,20 +6281,20 @@
       <selection activeCell="I31" sqref="A2:I31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="7.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.796875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.46484375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="104.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="104.46484375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="38" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="25.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25.46484375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
@@ -6221,7 +6323,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A2" s="7" t="s">
         <v>8</v>
       </c>
@@ -6250,7 +6352,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A3" s="7" t="s">
         <v>8</v>
       </c>
@@ -6279,7 +6381,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A4" s="7" t="s">
         <v>8</v>
       </c>
@@ -6308,7 +6410,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A5" s="7" t="s">
         <v>8</v>
       </c>
@@ -6337,7 +6439,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A6" s="7" t="s">
         <v>8</v>
       </c>
@@ -6366,7 +6468,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A7" s="7" t="s">
         <v>8</v>
       </c>
@@ -6395,7 +6497,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A8" s="7" t="s">
         <v>8</v>
       </c>
@@ -6424,7 +6526,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A9" s="7" t="s">
         <v>8</v>
       </c>
@@ -6453,7 +6555,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A10" s="7" t="s">
         <v>8</v>
       </c>
@@ -6482,7 +6584,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A11" s="7" t="s">
         <v>8</v>
       </c>
@@ -6511,7 +6613,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A12" s="7" t="s">
         <v>8</v>
       </c>
@@ -6540,7 +6642,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A13" s="7" t="s">
         <v>8</v>
       </c>
@@ -6569,7 +6671,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A14" s="7" t="s">
         <v>8</v>
       </c>
@@ -6598,7 +6700,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A15" s="7" t="s">
         <v>8</v>
       </c>
@@ -6627,7 +6729,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A16" s="7" t="s">
         <v>8</v>
       </c>
@@ -6656,7 +6758,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A17" s="7" t="s">
         <v>8</v>
       </c>
@@ -6685,7 +6787,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A18" s="7" t="s">
         <v>8</v>
       </c>
@@ -6714,7 +6816,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A19" s="7" t="s">
         <v>8</v>
       </c>
@@ -6743,7 +6845,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A20" s="7" t="s">
         <v>8</v>
       </c>
@@ -6772,7 +6874,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A21" s="7" t="s">
         <v>8</v>
       </c>
@@ -6801,7 +6903,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A22" s="7" t="s">
         <v>8</v>
       </c>
@@ -6830,7 +6932,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A23" s="7" t="s">
         <v>8</v>
       </c>
@@ -6859,7 +6961,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A24" s="7" t="s">
         <v>8</v>
       </c>
@@ -6888,7 +6990,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A25" s="7" t="s">
         <v>8</v>
       </c>
@@ -6917,7 +7019,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A26" s="7" t="s">
         <v>8</v>
       </c>
@@ -6946,7 +7048,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A27" s="7" t="s">
         <v>8</v>
       </c>
@@ -6975,7 +7077,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A28" s="7" t="s">
         <v>8</v>
       </c>
@@ -7004,7 +7106,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A29" s="7" t="s">
         <v>8</v>
       </c>
@@ -7033,7 +7135,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A30" s="7" t="s">
         <v>8</v>
       </c>
@@ -7062,7 +7164,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A31" s="7" t="s">
         <v>8</v>
       </c>
@@ -7091,7 +7193,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="32" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A32" s="15" t="s">
         <v>8</v>
       </c>
@@ -7120,7 +7222,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="33" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A33" s="15" t="s">
         <v>8</v>
       </c>
@@ -7149,7 +7251,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="34" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A34" s="15" t="s">
         <v>8</v>
       </c>
@@ -7178,7 +7280,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="35" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A35" s="20" t="s">
         <v>8</v>
       </c>
@@ -7207,7 +7309,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="36" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A36" s="20" t="s">
         <v>8</v>
       </c>
@@ -7236,7 +7338,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="37" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A37" s="21" t="s">
         <v>8</v>
       </c>
@@ -7265,7 +7367,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="38" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A38" s="20" t="s">
         <v>8</v>
       </c>
@@ -7294,7 +7396,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="39" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A39" s="22" t="s">
         <v>8</v>
       </c>
@@ -7323,7 +7425,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="40" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A40" s="15" t="s">
         <v>37</v>
       </c>
@@ -7352,7 +7454,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="41" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A41" s="15" t="s">
         <v>37</v>
       </c>
@@ -7381,7 +7483,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="42" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A42" s="15" t="s">
         <v>8</v>
       </c>
@@ -7410,7 +7512,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="43" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A43" s="15" t="s">
         <v>8</v>
       </c>
@@ -7439,7 +7541,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="44" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A44" s="15" t="s">
         <v>8</v>
       </c>
@@ -7468,7 +7570,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A45" s="9" t="s">
         <v>8</v>
       </c>
@@ -7495,7 +7597,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A46" s="7" t="s">
         <v>8</v>
       </c>
@@ -7520,7 +7622,7 @@
       </c>
       <c r="I46" s="7"/>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A47" s="8" t="s">
         <v>37</v>
       </c>
@@ -7549,7 +7651,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A48" s="8" t="s">
         <v>37</v>
       </c>
@@ -7576,7 +7678,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A49" s="9" t="s">
         <v>8</v>
       </c>
@@ -7605,7 +7707,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>

</xml_diff>

<commit_message>
Added NRSectorCarrier for 5G
</commit_message>
<xml_diff>
--- a/config/prod/RawFilePathCollection.xlsx
+++ b/config/prod/RawFilePathCollection.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Libraries\git\true\RanBaselineApp\source\config\prod\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46785452-BB43-45C6-9DA6-374EAD49CD21}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4343332F-A6B2-4BC8-804D-5FCC4CE9960D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{F32754BE-CF86-49F4-BEFD-53C8D448A04A}"/>
   </bookViews>
@@ -1250,8 +1250,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B114B3C2-9B56-4F69-A484-BA4ED1CFE527}">
   <dimension ref="A1:I65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D57" sqref="D57"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.19921875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>

<commit_message>
Add debug for ericsson
</commit_message>
<xml_diff>
--- a/config/prod/RawFilePathCollection.xlsx
+++ b/config/prod/RawFilePathCollection.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6e13cb156cc9c7c4/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Libraries\git\true\RanBaselineApp\source\config\prod\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="82" documentId="13_ncr:1_{4343332F-A6B2-4BC8-804D-5FCC4CE9960D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{D7F2A762-7852-40EF-A89A-181873530775}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D029D425-186E-4415-949C-17D3E46415E6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{F32754BE-CF86-49F4-BEFD-53C8D448A04A}"/>
   </bookViews>
@@ -1340,8 +1340,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B114B3C2-9B56-4F69-A484-BA4ED1CFE527}">
   <dimension ref="A1:I107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A78" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G97" sqref="G97"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.19921875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>

<commit_message>
Update huawei 4g path enbcfg
</commit_message>
<xml_diff>
--- a/config/prod/RawFilePathCollection.xlsx
+++ b/config/prod/RawFilePathCollection.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Libraries\git\true\RanBaselineApp\source\config\prod\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78F78B1C-A99B-450A-9D26-194A8C929688}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB5F8768-B632-474F-A354-58C1369EDF15}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{F32754BE-CF86-49F4-BEFD-53C8D448A04A}"/>
   </bookViews>
@@ -21,7 +21,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Backup!$A$1:$I$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Backup (2)'!$A$1:$I$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Path!$A$1:$I$73</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Path!$A$1:$I$93</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -204,7 +204,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1685" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1721" uniqueCount="217">
   <si>
     <t>ZTE</t>
   </si>
@@ -828,6 +828,33 @@
   </si>
   <si>
     <t>/home/app/ngoss/data/rfserver/UtranLTE/NOE/NodeB3900_8/1Current/</t>
+  </si>
+  <si>
+    <t>/home/app/ngoss/data/rfserver/UtranLTE/BMA/BTS3900_LTE1/1Current/</t>
+  </si>
+  <si>
+    <t>/home/app/ngoss/data/rfserver/UtranLTE/BMA/BTS3900_LTE2/1Current/</t>
+  </si>
+  <si>
+    <t>/home/app/ngoss/data/rfserver/UtranLTE/BMA/BTS3900_LTE3/1Current/</t>
+  </si>
+  <si>
+    <t>/home/app/ngoss/data/rfserver/UtranLTE/EAS/BTS3900_LTE1/1Current/</t>
+  </si>
+  <si>
+    <t>/home/app/ngoss/data/rfserver/UtranLTE/EAS/BTS3900_LTE2/1Current/</t>
+  </si>
+  <si>
+    <t>/home/app/ngoss/data/rfserver/UtranLTE/EAS/BTS3900_LTE3/1Current/</t>
+  </si>
+  <si>
+    <t>/home/app/ngoss/data/rfserver/UtranLTE/NOE/BTS3900_LTE1/1Current/</t>
+  </si>
+  <si>
+    <t>/home/app/ngoss/data/rfserver/UtranLTE/NOE/BTS3900_LTE2/1Current/</t>
+  </si>
+  <si>
+    <t>/home/app/ngoss/data/rfserver/UtranLTE/NOE/BTS3900_LTE3/1Current/</t>
   </si>
 </sst>
 </file>
@@ -1361,10 +1388,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B114B3C2-9B56-4F69-A484-BA4ED1CFE527}">
-  <dimension ref="A1:I89"/>
+  <dimension ref="A1:I93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A59" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G89" sqref="G89"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.19921875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1777,7 +1804,7 @@
         <v>13</v>
       </c>
       <c r="G14" s="24" t="s">
-        <v>71</v>
+        <v>208</v>
       </c>
       <c r="H14" s="24" t="s">
         <v>39</v>
@@ -1806,7 +1833,7 @@
         <v>13</v>
       </c>
       <c r="G15" s="24" t="s">
-        <v>72</v>
+        <v>209</v>
       </c>
       <c r="H15" s="24" t="s">
         <v>39</v>
@@ -1835,7 +1862,7 @@
         <v>13</v>
       </c>
       <c r="G16" s="24" t="s">
-        <v>73</v>
+        <v>210</v>
       </c>
       <c r="H16" s="24" t="s">
         <v>39</v>
@@ -1864,7 +1891,7 @@
         <v>13</v>
       </c>
       <c r="G17" s="24" t="s">
-        <v>74</v>
+        <v>211</v>
       </c>
       <c r="H17" s="24" t="s">
         <v>39</v>
@@ -1887,13 +1914,13 @@
         <v>33</v>
       </c>
       <c r="E18" s="29" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F18" s="29" t="s">
         <v>13</v>
       </c>
       <c r="G18" s="24" t="s">
-        <v>75</v>
+        <v>212</v>
       </c>
       <c r="H18" s="24" t="s">
         <v>39</v>
@@ -1904,60 +1931,60 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A19" s="29" t="s">
-        <v>37</v>
+        <v>8</v>
       </c>
       <c r="B19" s="24" t="s">
         <v>9</v>
       </c>
       <c r="C19" s="24" t="s">
-        <v>1</v>
-      </c>
-      <c r="D19" s="29">
-        <v>850</v>
+        <v>16</v>
+      </c>
+      <c r="D19" s="29" t="s">
+        <v>33</v>
       </c>
       <c r="E19" s="29" t="s">
-        <v>34</v>
+        <v>57</v>
       </c>
       <c r="F19" s="29" t="s">
         <v>13</v>
       </c>
       <c r="G19" s="24" t="s">
-        <v>66</v>
+        <v>213</v>
       </c>
       <c r="H19" s="24" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="I19" s="29" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A20" s="29" t="s">
-        <v>37</v>
+        <v>8</v>
       </c>
       <c r="B20" s="24" t="s">
         <v>9</v>
       </c>
       <c r="C20" s="24" t="s">
-        <v>1</v>
-      </c>
-      <c r="D20" s="29">
-        <v>850</v>
+        <v>16</v>
+      </c>
+      <c r="D20" s="29" t="s">
+        <v>33</v>
       </c>
       <c r="E20" s="29" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F20" s="29" t="s">
         <v>13</v>
       </c>
       <c r="G20" s="24" t="s">
-        <v>67</v>
+        <v>214</v>
       </c>
       <c r="H20" s="24" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="I20" s="29" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.45">
@@ -1968,25 +1995,25 @@
         <v>9</v>
       </c>
       <c r="C21" s="24" t="s">
-        <v>1</v>
-      </c>
-      <c r="D21" s="29">
-        <v>2100</v>
+        <v>16</v>
+      </c>
+      <c r="D21" s="29" t="s">
+        <v>33</v>
       </c>
       <c r="E21" s="29" t="s">
-        <v>34</v>
+        <v>58</v>
       </c>
       <c r="F21" s="29" t="s">
         <v>13</v>
       </c>
       <c r="G21" s="24" t="s">
-        <v>68</v>
+        <v>215</v>
       </c>
       <c r="H21" s="24" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="I21" s="29" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.45">
@@ -1997,30 +2024,30 @@
         <v>9</v>
       </c>
       <c r="C22" s="24" t="s">
-        <v>1</v>
-      </c>
-      <c r="D22" s="29">
-        <v>2100</v>
+        <v>16</v>
+      </c>
+      <c r="D22" s="29" t="s">
+        <v>33</v>
       </c>
       <c r="E22" s="29" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="F22" s="29" t="s">
         <v>13</v>
       </c>
       <c r="G22" s="24" t="s">
-        <v>69</v>
+        <v>216</v>
       </c>
       <c r="H22" s="24" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="I22" s="29" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A23" s="29" t="s">
-        <v>8</v>
+        <v>37</v>
       </c>
       <c r="B23" s="24" t="s">
         <v>9</v>
@@ -2029,16 +2056,16 @@
         <v>1</v>
       </c>
       <c r="D23" s="29">
-        <v>2100</v>
+        <v>850</v>
       </c>
       <c r="E23" s="29" t="s">
-        <v>58</v>
+        <v>34</v>
       </c>
       <c r="F23" s="29" t="s">
         <v>13</v>
       </c>
       <c r="G23" s="24" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="H23" s="24" t="s">
         <v>35</v>
@@ -2049,29 +2076,31 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A24" s="29" t="s">
-        <v>8</v>
+        <v>37</v>
       </c>
       <c r="B24" s="24" t="s">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="C24" s="24" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="D24" s="29">
-        <v>900</v>
-      </c>
-      <c r="E24" s="29"/>
+        <v>850</v>
+      </c>
+      <c r="E24" s="29" t="s">
+        <v>59</v>
+      </c>
       <c r="F24" s="29" t="s">
         <v>13</v>
       </c>
       <c r="G24" s="24" t="s">
-        <v>80</v>
+        <v>67</v>
       </c>
       <c r="H24" s="24" t="s">
-        <v>159</v>
+        <v>35</v>
       </c>
       <c r="I24" s="29" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.45">
@@ -2079,80 +2108,86 @@
         <v>8</v>
       </c>
       <c r="B25" s="24" t="s">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="C25" s="24" t="s">
-        <v>16</v>
-      </c>
-      <c r="D25" s="29" t="s">
-        <v>33</v>
-      </c>
-      <c r="E25" s="29"/>
+        <v>1</v>
+      </c>
+      <c r="D25" s="29">
+        <v>2100</v>
+      </c>
+      <c r="E25" s="29" t="s">
+        <v>34</v>
+      </c>
       <c r="F25" s="29" t="s">
         <v>13</v>
       </c>
       <c r="G25" s="24" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="H25" s="24" t="s">
-        <v>160</v>
-      </c>
-      <c r="I25" s="29"/>
+        <v>35</v>
+      </c>
+      <c r="I25" s="29" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A26" s="29" t="s">
-        <v>37</v>
+        <v>8</v>
       </c>
       <c r="B26" s="24" t="s">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="C26" s="24" t="s">
         <v>1</v>
       </c>
       <c r="D26" s="29">
-        <v>850</v>
+        <v>2100</v>
       </c>
       <c r="E26" s="29" t="s">
-        <v>43</v>
+        <v>57</v>
       </c>
       <c r="F26" s="29" t="s">
         <v>13</v>
       </c>
       <c r="G26" s="24" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="H26" s="24" t="s">
-        <v>161</v>
+        <v>35</v>
       </c>
       <c r="I26" s="29" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A27" s="29" t="s">
-        <v>37</v>
+        <v>8</v>
       </c>
       <c r="B27" s="24" t="s">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="C27" s="24" t="s">
         <v>1</v>
       </c>
       <c r="D27" s="29">
-        <v>850</v>
-      </c>
-      <c r="E27" s="29"/>
+        <v>2100</v>
+      </c>
+      <c r="E27" s="29" t="s">
+        <v>58</v>
+      </c>
       <c r="F27" s="29" t="s">
         <v>13</v>
       </c>
       <c r="G27" s="24" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="H27" s="24" t="s">
-        <v>161</v>
+        <v>35</v>
       </c>
       <c r="I27" s="29" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.45">
@@ -2163,14 +2198,12 @@
         <v>0</v>
       </c>
       <c r="C28" s="24" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="D28" s="29">
-        <v>2100</v>
-      </c>
-      <c r="E28" s="29" t="s">
-        <v>46</v>
-      </c>
+        <v>900</v>
+      </c>
+      <c r="E28" s="29"/>
       <c r="F28" s="29" t="s">
         <v>13</v>
       </c>
@@ -2178,10 +2211,10 @@
         <v>80</v>
       </c>
       <c r="H28" s="24" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="I28" s="29" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.45">
@@ -2189,86 +2222,80 @@
         <v>8</v>
       </c>
       <c r="B29" s="24" t="s">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="C29" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="D29" s="29">
-        <v>900</v>
-      </c>
-      <c r="E29" s="29" t="s">
-        <v>55</v>
-      </c>
+      <c r="D29" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="E29" s="29"/>
       <c r="F29" s="29" t="s">
         <v>13</v>
       </c>
       <c r="G29" s="24" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="H29" s="24" t="s">
-        <v>51</v>
-      </c>
-      <c r="I29" s="29" t="s">
-        <v>53</v>
-      </c>
+        <v>160</v>
+      </c>
+      <c r="I29" s="29"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A30" s="29" t="s">
-        <v>8</v>
+        <v>37</v>
       </c>
       <c r="B30" s="24" t="s">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="C30" s="24" t="s">
-        <v>16</v>
-      </c>
-      <c r="D30" s="29" t="s">
-        <v>54</v>
+        <v>1</v>
+      </c>
+      <c r="D30" s="29">
+        <v>850</v>
       </c>
       <c r="E30" s="29" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="F30" s="29" t="s">
         <v>13</v>
       </c>
       <c r="G30" s="24" t="s">
-        <v>90</v>
+        <v>77</v>
       </c>
       <c r="H30" s="24" t="s">
-        <v>51</v>
+        <v>161</v>
       </c>
       <c r="I30" s="29" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A31" s="29" t="s">
-        <v>8</v>
+        <v>37</v>
       </c>
       <c r="B31" s="24" t="s">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="C31" s="24" t="s">
-        <v>16</v>
-      </c>
-      <c r="D31" s="29" t="s">
-        <v>54</v>
-      </c>
-      <c r="E31" s="29" t="s">
-        <v>55</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="D31" s="29">
+        <v>850</v>
+      </c>
+      <c r="E31" s="29"/>
       <c r="F31" s="29" t="s">
         <v>13</v>
       </c>
       <c r="G31" s="24" t="s">
-        <v>162</v>
+        <v>78</v>
       </c>
       <c r="H31" s="24" t="s">
-        <v>51</v>
+        <v>161</v>
       </c>
       <c r="I31" s="29" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.45">
@@ -2276,28 +2303,28 @@
         <v>8</v>
       </c>
       <c r="B32" s="24" t="s">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="C32" s="24" t="s">
-        <v>16</v>
-      </c>
-      <c r="D32" s="29" t="s">
-        <v>54</v>
+        <v>1</v>
+      </c>
+      <c r="D32" s="29">
+        <v>2100</v>
       </c>
       <c r="E32" s="29" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="F32" s="29" t="s">
         <v>13</v>
       </c>
       <c r="G32" s="24" t="s">
-        <v>167</v>
+        <v>80</v>
       </c>
       <c r="H32" s="24" t="s">
-        <v>51</v>
+        <v>161</v>
       </c>
       <c r="I32" s="29" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.45">
@@ -2310,8 +2337,8 @@
       <c r="C33" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="D33" s="29" t="s">
-        <v>54</v>
+      <c r="D33" s="29">
+        <v>900</v>
       </c>
       <c r="E33" s="29" t="s">
         <v>55</v>
@@ -2320,7 +2347,7 @@
         <v>13</v>
       </c>
       <c r="G33" s="24" t="s">
-        <v>168</v>
+        <v>89</v>
       </c>
       <c r="H33" s="24" t="s">
         <v>51</v>
@@ -2337,10 +2364,10 @@
         <v>17</v>
       </c>
       <c r="C34" s="24" t="s">
-        <v>1</v>
-      </c>
-      <c r="D34" s="29">
-        <v>2100</v>
+        <v>16</v>
+      </c>
+      <c r="D34" s="29" t="s">
+        <v>54</v>
       </c>
       <c r="E34" s="29" t="s">
         <v>55</v>
@@ -2349,7 +2376,7 @@
         <v>13</v>
       </c>
       <c r="G34" s="24" t="s">
-        <v>169</v>
+        <v>90</v>
       </c>
       <c r="H34" s="24" t="s">
         <v>51</v>
@@ -2366,10 +2393,10 @@
         <v>17</v>
       </c>
       <c r="C35" s="24" t="s">
-        <v>1</v>
-      </c>
-      <c r="D35" s="29">
-        <v>2100</v>
+        <v>16</v>
+      </c>
+      <c r="D35" s="29" t="s">
+        <v>54</v>
       </c>
       <c r="E35" s="29" t="s">
         <v>55</v>
@@ -2378,7 +2405,7 @@
         <v>13</v>
       </c>
       <c r="G35" s="24" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="H35" s="24" t="s">
         <v>51</v>
@@ -2395,10 +2422,10 @@
         <v>17</v>
       </c>
       <c r="C36" s="24" t="s">
-        <v>1</v>
-      </c>
-      <c r="D36" s="29">
-        <v>2100</v>
+        <v>16</v>
+      </c>
+      <c r="D36" s="29" t="s">
+        <v>54</v>
       </c>
       <c r="E36" s="29" t="s">
         <v>55</v>
@@ -2407,7 +2434,7 @@
         <v>13</v>
       </c>
       <c r="G36" s="24" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="H36" s="24" t="s">
         <v>51</v>
@@ -2424,10 +2451,10 @@
         <v>17</v>
       </c>
       <c r="C37" s="24" t="s">
-        <v>1</v>
-      </c>
-      <c r="D37" s="29">
-        <v>2100</v>
+        <v>16</v>
+      </c>
+      <c r="D37" s="29" t="s">
+        <v>54</v>
       </c>
       <c r="E37" s="29" t="s">
         <v>55</v>
@@ -2436,7 +2463,7 @@
         <v>13</v>
       </c>
       <c r="G37" s="24" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="H37" s="24" t="s">
         <v>51</v>
@@ -2465,7 +2492,7 @@
         <v>13</v>
       </c>
       <c r="G38" s="24" t="s">
-        <v>162</v>
+        <v>169</v>
       </c>
       <c r="H38" s="24" t="s">
         <v>51</v>
@@ -2494,7 +2521,7 @@
         <v>13</v>
       </c>
       <c r="G39" s="24" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="H39" s="24" t="s">
         <v>51</v>
@@ -2511,10 +2538,10 @@
         <v>17</v>
       </c>
       <c r="C40" s="24" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="D40" s="29">
-        <v>900</v>
+        <v>2100</v>
       </c>
       <c r="E40" s="29" t="s">
         <v>55</v>
@@ -2523,13 +2550,13 @@
         <v>13</v>
       </c>
       <c r="G40" s="24" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="H40" s="24" t="s">
         <v>51</v>
       </c>
       <c r="I40" s="29" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.45">
@@ -2540,10 +2567,10 @@
         <v>17</v>
       </c>
       <c r="C41" s="24" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="D41" s="29">
-        <v>900</v>
+        <v>2100</v>
       </c>
       <c r="E41" s="29" t="s">
         <v>55</v>
@@ -2558,7 +2585,7 @@
         <v>51</v>
       </c>
       <c r="I41" s="29" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.45">
@@ -2569,10 +2596,10 @@
         <v>17</v>
       </c>
       <c r="C42" s="24" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="D42" s="29">
-        <v>900</v>
+        <v>2100</v>
       </c>
       <c r="E42" s="29" t="s">
         <v>55</v>
@@ -2581,13 +2608,13 @@
         <v>13</v>
       </c>
       <c r="G42" s="24" t="s">
-        <v>174</v>
+        <v>162</v>
       </c>
       <c r="H42" s="24" t="s">
         <v>51</v>
       </c>
       <c r="I42" s="29" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.45">
@@ -2598,10 +2625,10 @@
         <v>17</v>
       </c>
       <c r="C43" s="24" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="D43" s="29">
-        <v>900</v>
+        <v>2100</v>
       </c>
       <c r="E43" s="29" t="s">
         <v>55</v>
@@ -2616,7 +2643,7 @@
         <v>51</v>
       </c>
       <c r="I43" s="29" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.45">
@@ -2627,25 +2654,25 @@
         <v>17</v>
       </c>
       <c r="C44" s="24" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="D44" s="29">
         <v>900</v>
       </c>
       <c r="E44" s="29" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="F44" s="29" t="s">
         <v>13</v>
       </c>
       <c r="G44" s="24" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="H44" s="24" t="s">
         <v>51</v>
       </c>
       <c r="I44" s="29" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.45">
@@ -2656,25 +2683,25 @@
         <v>17</v>
       </c>
       <c r="C45" s="24" t="s">
-        <v>16</v>
-      </c>
-      <c r="D45" s="29" t="s">
-        <v>54</v>
+        <v>11</v>
+      </c>
+      <c r="D45" s="29">
+        <v>900</v>
       </c>
       <c r="E45" s="29" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="F45" s="29" t="s">
         <v>13</v>
       </c>
       <c r="G45" s="24" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="H45" s="24" t="s">
         <v>51</v>
       </c>
       <c r="I45" s="29" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.45">
@@ -2685,25 +2712,25 @@
         <v>17</v>
       </c>
       <c r="C46" s="24" t="s">
-        <v>16</v>
-      </c>
-      <c r="D46" s="29" t="s">
-        <v>54</v>
+        <v>11</v>
+      </c>
+      <c r="D46" s="29">
+        <v>900</v>
       </c>
       <c r="E46" s="29" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="F46" s="29" t="s">
         <v>13</v>
       </c>
       <c r="G46" s="24" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="H46" s="24" t="s">
         <v>51</v>
       </c>
       <c r="I46" s="29" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.45">
@@ -2714,25 +2741,25 @@
         <v>17</v>
       </c>
       <c r="C47" s="24" t="s">
-        <v>16</v>
-      </c>
-      <c r="D47" s="29" t="s">
-        <v>54</v>
+        <v>11</v>
+      </c>
+      <c r="D47" s="29">
+        <v>900</v>
       </c>
       <c r="E47" s="29" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="F47" s="29" t="s">
         <v>13</v>
       </c>
       <c r="G47" s="24" t="s">
-        <v>178</v>
+        <v>167</v>
       </c>
       <c r="H47" s="24" t="s">
         <v>51</v>
       </c>
       <c r="I47" s="29" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.45">
@@ -2745,8 +2772,8 @@
       <c r="C48" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="D48" s="29" t="s">
-        <v>54</v>
+      <c r="D48" s="29">
+        <v>900</v>
       </c>
       <c r="E48" s="29" t="s">
         <v>46</v>
@@ -2755,7 +2782,7 @@
         <v>13</v>
       </c>
       <c r="G48" s="24" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="H48" s="24" t="s">
         <v>51</v>
@@ -2772,10 +2799,10 @@
         <v>17</v>
       </c>
       <c r="C49" s="24" t="s">
-        <v>1</v>
-      </c>
-      <c r="D49" s="29">
-        <v>2100</v>
+        <v>16</v>
+      </c>
+      <c r="D49" s="29" t="s">
+        <v>54</v>
       </c>
       <c r="E49" s="29" t="s">
         <v>46</v>
@@ -2784,7 +2811,7 @@
         <v>13</v>
       </c>
       <c r="G49" s="24" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="H49" s="24" t="s">
         <v>51</v>
@@ -2801,10 +2828,10 @@
         <v>17</v>
       </c>
       <c r="C50" s="24" t="s">
-        <v>1</v>
-      </c>
-      <c r="D50" s="29">
-        <v>2100</v>
+        <v>16</v>
+      </c>
+      <c r="D50" s="29" t="s">
+        <v>54</v>
       </c>
       <c r="E50" s="29" t="s">
         <v>46</v>
@@ -2813,7 +2840,7 @@
         <v>13</v>
       </c>
       <c r="G50" s="24" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="H50" s="24" t="s">
         <v>51</v>
@@ -2830,10 +2857,10 @@
         <v>17</v>
       </c>
       <c r="C51" s="24" t="s">
-        <v>1</v>
-      </c>
-      <c r="D51" s="29">
-        <v>2100</v>
+        <v>16</v>
+      </c>
+      <c r="D51" s="29" t="s">
+        <v>54</v>
       </c>
       <c r="E51" s="29" t="s">
         <v>46</v>
@@ -2842,7 +2869,7 @@
         <v>13</v>
       </c>
       <c r="G51" s="24" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="H51" s="24" t="s">
         <v>51</v>
@@ -2859,10 +2886,10 @@
         <v>17</v>
       </c>
       <c r="C52" s="24" t="s">
-        <v>1</v>
-      </c>
-      <c r="D52" s="29">
-        <v>2100</v>
+        <v>16</v>
+      </c>
+      <c r="D52" s="29" t="s">
+        <v>54</v>
       </c>
       <c r="E52" s="29" t="s">
         <v>46</v>
@@ -2871,7 +2898,7 @@
         <v>13</v>
       </c>
       <c r="G52" s="24" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="H52" s="24" t="s">
         <v>51</v>
@@ -2900,7 +2927,7 @@
         <v>13</v>
       </c>
       <c r="G53" s="24" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="H53" s="24" t="s">
         <v>51</v>
@@ -2929,7 +2956,7 @@
         <v>13</v>
       </c>
       <c r="G54" s="24" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="H54" s="24" t="s">
         <v>51</v>
@@ -2946,10 +2973,10 @@
         <v>17</v>
       </c>
       <c r="C55" s="24" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="D55" s="29">
-        <v>900</v>
+        <v>2100</v>
       </c>
       <c r="E55" s="29" t="s">
         <v>46</v>
@@ -2958,13 +2985,13 @@
         <v>13</v>
       </c>
       <c r="G55" s="24" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="H55" s="24" t="s">
         <v>51</v>
       </c>
       <c r="I55" s="29" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.45">
@@ -2975,10 +3002,10 @@
         <v>17</v>
       </c>
       <c r="C56" s="24" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="D56" s="29">
-        <v>900</v>
+        <v>2100</v>
       </c>
       <c r="E56" s="29" t="s">
         <v>46</v>
@@ -2993,7 +3020,7 @@
         <v>51</v>
       </c>
       <c r="I56" s="29" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.45">
@@ -3004,10 +3031,10 @@
         <v>17</v>
       </c>
       <c r="C57" s="24" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="D57" s="29">
-        <v>900</v>
+        <v>2100</v>
       </c>
       <c r="E57" s="29" t="s">
         <v>46</v>
@@ -3016,13 +3043,13 @@
         <v>13</v>
       </c>
       <c r="G57" s="24" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
       <c r="H57" s="24" t="s">
         <v>51</v>
       </c>
       <c r="I57" s="29" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.45">
@@ -3033,10 +3060,10 @@
         <v>17</v>
       </c>
       <c r="C58" s="24" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="D58" s="29">
-        <v>900</v>
+        <v>2100</v>
       </c>
       <c r="E58" s="29" t="s">
         <v>46</v>
@@ -3051,7 +3078,7 @@
         <v>51</v>
       </c>
       <c r="I58" s="29" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.45">
@@ -3062,25 +3089,25 @@
         <v>17</v>
       </c>
       <c r="C59" s="24" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="D59" s="29">
         <v>900</v>
       </c>
       <c r="E59" s="29" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F59" s="29" t="s">
         <v>13</v>
       </c>
       <c r="G59" s="24" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="H59" s="24" t="s">
         <v>51</v>
       </c>
       <c r="I59" s="29" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.45">
@@ -3091,25 +3118,25 @@
         <v>17</v>
       </c>
       <c r="C60" s="24" t="s">
-        <v>16</v>
-      </c>
-      <c r="D60" s="29" t="s">
-        <v>54</v>
+        <v>11</v>
+      </c>
+      <c r="D60" s="29">
+        <v>900</v>
       </c>
       <c r="E60" s="29" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F60" s="29" t="s">
         <v>13</v>
       </c>
       <c r="G60" s="24" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="H60" s="24" t="s">
         <v>51</v>
       </c>
       <c r="I60" s="29" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.45">
@@ -3120,25 +3147,25 @@
         <v>17</v>
       </c>
       <c r="C61" s="24" t="s">
-        <v>16</v>
-      </c>
-      <c r="D61" s="29" t="s">
-        <v>54</v>
+        <v>11</v>
+      </c>
+      <c r="D61" s="29">
+        <v>900</v>
       </c>
       <c r="E61" s="29" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F61" s="29" t="s">
         <v>13</v>
       </c>
       <c r="G61" s="24" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="H61" s="24" t="s">
         <v>51</v>
       </c>
       <c r="I61" s="29" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.45">
@@ -3149,25 +3176,25 @@
         <v>17</v>
       </c>
       <c r="C62" s="24" t="s">
-        <v>16</v>
-      </c>
-      <c r="D62" s="29" t="s">
-        <v>54</v>
+        <v>11</v>
+      </c>
+      <c r="D62" s="29">
+        <v>900</v>
       </c>
       <c r="E62" s="29" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F62" s="29" t="s">
         <v>13</v>
       </c>
       <c r="G62" s="24" t="s">
-        <v>189</v>
+        <v>178</v>
       </c>
       <c r="H62" s="24" t="s">
         <v>51</v>
       </c>
       <c r="I62" s="29" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.45">
@@ -3180,8 +3207,8 @@
       <c r="C63" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="D63" s="29" t="s">
-        <v>54</v>
+      <c r="D63" s="29">
+        <v>900</v>
       </c>
       <c r="E63" s="29" t="s">
         <v>48</v>
@@ -3190,7 +3217,7 @@
         <v>13</v>
       </c>
       <c r="G63" s="24" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="H63" s="24" t="s">
         <v>51</v>
@@ -3207,10 +3234,10 @@
         <v>17</v>
       </c>
       <c r="C64" s="24" t="s">
-        <v>1</v>
-      </c>
-      <c r="D64" s="29">
-        <v>2100</v>
+        <v>16</v>
+      </c>
+      <c r="D64" s="29" t="s">
+        <v>54</v>
       </c>
       <c r="E64" s="29" t="s">
         <v>48</v>
@@ -3219,7 +3246,7 @@
         <v>13</v>
       </c>
       <c r="G64" s="24" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="H64" s="24" t="s">
         <v>51</v>
@@ -3236,10 +3263,10 @@
         <v>17</v>
       </c>
       <c r="C65" s="24" t="s">
-        <v>1</v>
-      </c>
-      <c r="D65" s="29">
-        <v>2100</v>
+        <v>16</v>
+      </c>
+      <c r="D65" s="29" t="s">
+        <v>54</v>
       </c>
       <c r="E65" s="29" t="s">
         <v>48</v>
@@ -3248,7 +3275,7 @@
         <v>13</v>
       </c>
       <c r="G65" s="24" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="H65" s="24" t="s">
         <v>51</v>
@@ -3265,10 +3292,10 @@
         <v>17</v>
       </c>
       <c r="C66" s="24" t="s">
-        <v>1</v>
-      </c>
-      <c r="D66" s="29">
-        <v>2100</v>
+        <v>16</v>
+      </c>
+      <c r="D66" s="29" t="s">
+        <v>54</v>
       </c>
       <c r="E66" s="29" t="s">
         <v>48</v>
@@ -3277,7 +3304,7 @@
         <v>13</v>
       </c>
       <c r="G66" s="24" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="H66" s="24" t="s">
         <v>51</v>
@@ -3294,10 +3321,10 @@
         <v>17</v>
       </c>
       <c r="C67" s="24" t="s">
-        <v>1</v>
-      </c>
-      <c r="D67" s="29">
-        <v>2100</v>
+        <v>16</v>
+      </c>
+      <c r="D67" s="29" t="s">
+        <v>54</v>
       </c>
       <c r="E67" s="29" t="s">
         <v>48</v>
@@ -3306,7 +3333,7 @@
         <v>13</v>
       </c>
       <c r="G67" s="24" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="H67" s="24" t="s">
         <v>51</v>
@@ -3335,7 +3362,7 @@
         <v>13</v>
       </c>
       <c r="G68" s="24" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="H68" s="24" t="s">
         <v>51</v>
@@ -3364,7 +3391,7 @@
         <v>13</v>
       </c>
       <c r="G69" s="24" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="H69" s="24" t="s">
         <v>51</v>
@@ -3381,10 +3408,10 @@
         <v>17</v>
       </c>
       <c r="C70" s="24" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="D70" s="29">
-        <v>900</v>
+        <v>2100</v>
       </c>
       <c r="E70" s="29" t="s">
         <v>48</v>
@@ -3393,13 +3420,13 @@
         <v>13</v>
       </c>
       <c r="G70" s="24" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="H70" s="24" t="s">
         <v>51</v>
       </c>
       <c r="I70" s="29" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.45">
@@ -3410,10 +3437,10 @@
         <v>17</v>
       </c>
       <c r="C71" s="24" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="D71" s="29">
-        <v>900</v>
+        <v>2100</v>
       </c>
       <c r="E71" s="29" t="s">
         <v>48</v>
@@ -3428,7 +3455,7 @@
         <v>51</v>
       </c>
       <c r="I71" s="29" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.45">
@@ -3439,10 +3466,10 @@
         <v>17</v>
       </c>
       <c r="C72" s="24" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="D72" s="29">
-        <v>900</v>
+        <v>2100</v>
       </c>
       <c r="E72" s="29" t="s">
         <v>48</v>
@@ -3451,13 +3478,13 @@
         <v>13</v>
       </c>
       <c r="G72" s="24" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="H72" s="24" t="s">
         <v>51</v>
       </c>
       <c r="I72" s="29" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.45">
@@ -3468,10 +3495,10 @@
         <v>17</v>
       </c>
       <c r="C73" s="24" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="D73" s="29">
-        <v>900</v>
+        <v>2100</v>
       </c>
       <c r="E73" s="29" t="s">
         <v>48</v>
@@ -3486,150 +3513,158 @@
         <v>51</v>
       </c>
       <c r="I73" s="29" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A74" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="B74" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="C74" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="D74" s="29">
+        <v>900</v>
+      </c>
+      <c r="E74" s="29" t="s">
+        <v>48</v>
+      </c>
+      <c r="F74" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="G74" s="24" t="s">
+        <v>195</v>
+      </c>
+      <c r="H74" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="I74" s="29" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="74" spans="1:9" s="30" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A74" s="29" t="s">
-        <v>8</v>
-      </c>
-      <c r="B74" s="24" t="s">
-        <v>0</v>
-      </c>
-      <c r="C74" s="24" t="s">
-        <v>163</v>
-      </c>
-      <c r="D74" s="29">
-        <v>2600</v>
-      </c>
-      <c r="E74" s="29" t="s">
-        <v>46</v>
-      </c>
-      <c r="F74" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="G74" s="24" t="s">
-        <v>197</v>
-      </c>
-      <c r="H74" s="24" t="s">
-        <v>202</v>
-      </c>
-      <c r="I74" s="29"/>
-    </row>
-    <row r="75" spans="1:9" s="30" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A75" s="29" t="s">
         <v>8</v>
       </c>
       <c r="B75" s="24" t="s">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="C75" s="24" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="D75" s="29">
-        <v>2600</v>
+        <v>900</v>
       </c>
       <c r="E75" s="29" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="F75" s="29" t="s">
         <v>13</v>
       </c>
       <c r="G75" s="24" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="H75" s="24" t="s">
-        <v>202</v>
-      </c>
-      <c r="I75" s="29"/>
+        <v>51</v>
+      </c>
+      <c r="I75" s="29" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A76" s="29" t="s">
         <v>8</v>
       </c>
       <c r="B76" s="24" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="C76" s="24" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="D76" s="29">
-        <v>2600</v>
+        <v>900</v>
       </c>
       <c r="E76" s="29" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="F76" s="29" t="s">
         <v>13</v>
       </c>
       <c r="G76" s="24" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="H76" s="24" t="s">
-        <v>203</v>
-      </c>
-      <c r="I76" s="29"/>
+        <v>51</v>
+      </c>
+      <c r="I76" s="29" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A77" s="29" t="s">
         <v>8</v>
       </c>
       <c r="B77" s="24" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="C77" s="24" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="D77" s="29">
-        <v>2600</v>
+        <v>900</v>
       </c>
       <c r="E77" s="29" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="F77" s="29" t="s">
         <v>13</v>
       </c>
       <c r="G77" s="24" t="s">
-        <v>199</v>
+        <v>189</v>
       </c>
       <c r="H77" s="24" t="s">
-        <v>203</v>
-      </c>
-      <c r="I77" s="29"/>
-    </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.45">
+        <v>51</v>
+      </c>
+      <c r="I77" s="29" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" s="30" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A78" s="29" t="s">
         <v>8</v>
       </c>
       <c r="B78" s="24" t="s">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="C78" s="24" t="s">
-        <v>16</v>
+        <v>163</v>
       </c>
       <c r="D78" s="29">
         <v>2600</v>
       </c>
       <c r="E78" s="29" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
       <c r="F78" s="29" t="s">
         <v>13</v>
       </c>
       <c r="G78" s="24" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="H78" s="24" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="I78" s="29"/>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:9" s="30" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A79" s="29" t="s">
         <v>8</v>
       </c>
       <c r="B79" s="24" t="s">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="C79" s="24" t="s">
         <v>16</v>
@@ -3638,16 +3673,16 @@
         <v>2600</v>
       </c>
       <c r="E79" s="29" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
       <c r="F79" s="29" t="s">
         <v>13</v>
       </c>
       <c r="G79" s="24" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="H79" s="24" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="I79" s="29"/>
     </row>
@@ -3661,17 +3696,17 @@
       <c r="C80" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="D80" s="29" t="s">
-        <v>204</v>
+      <c r="D80" s="29">
+        <v>2600</v>
       </c>
       <c r="E80" s="29" t="s">
-        <v>58</v>
+        <v>34</v>
       </c>
       <c r="F80" s="29" t="s">
         <v>13</v>
       </c>
       <c r="G80" s="24" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="H80" s="24" t="s">
         <v>203</v>
@@ -3688,17 +3723,17 @@
       <c r="C81" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="D81" s="29" t="s">
-        <v>204</v>
+      <c r="D81" s="29">
+        <v>2600</v>
       </c>
       <c r="E81" s="29" t="s">
-        <v>58</v>
+        <v>34</v>
       </c>
       <c r="F81" s="29" t="s">
         <v>13</v>
       </c>
       <c r="G81" s="24" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
       <c r="H81" s="24" t="s">
         <v>203</v>
@@ -3715,17 +3750,17 @@
       <c r="C82" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="D82" s="29" t="s">
-        <v>204</v>
+      <c r="D82" s="29">
+        <v>2600</v>
       </c>
       <c r="E82" s="29" t="s">
-        <v>58</v>
+        <v>34</v>
       </c>
       <c r="F82" s="29" t="s">
         <v>13</v>
       </c>
       <c r="G82" s="24" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="H82" s="24" t="s">
         <v>203</v>
@@ -3740,7 +3775,7 @@
         <v>9</v>
       </c>
       <c r="C83" s="24" t="s">
-        <v>163</v>
+        <v>16</v>
       </c>
       <c r="D83" s="29">
         <v>2600</v>
@@ -3752,7 +3787,7 @@
         <v>13</v>
       </c>
       <c r="G83" s="24" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="H83" s="24" t="s">
         <v>203</v>
@@ -3767,19 +3802,19 @@
         <v>9</v>
       </c>
       <c r="C84" s="24" t="s">
-        <v>163</v>
-      </c>
-      <c r="D84" s="29">
-        <v>2600</v>
+        <v>16</v>
+      </c>
+      <c r="D84" s="29" t="s">
+        <v>204</v>
       </c>
       <c r="E84" s="29" t="s">
-        <v>34</v>
+        <v>58</v>
       </c>
       <c r="F84" s="29" t="s">
         <v>13</v>
       </c>
       <c r="G84" s="24" t="s">
-        <v>199</v>
+        <v>205</v>
       </c>
       <c r="H84" s="24" t="s">
         <v>203</v>
@@ -3794,26 +3829,26 @@
         <v>9</v>
       </c>
       <c r="C85" s="24" t="s">
-        <v>163</v>
-      </c>
-      <c r="D85" s="29">
-        <v>2600</v>
+        <v>16</v>
+      </c>
+      <c r="D85" s="29" t="s">
+        <v>204</v>
       </c>
       <c r="E85" s="29" t="s">
-        <v>34</v>
+        <v>58</v>
       </c>
       <c r="F85" s="29" t="s">
         <v>13</v>
       </c>
       <c r="G85" s="24" t="s">
-        <v>200</v>
+        <v>206</v>
       </c>
       <c r="H85" s="24" t="s">
         <v>203</v>
       </c>
       <c r="I85" s="29"/>
     </row>
-    <row r="86" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A86" s="29" t="s">
         <v>8</v>
       </c>
@@ -3821,19 +3856,19 @@
         <v>9</v>
       </c>
       <c r="C86" s="24" t="s">
-        <v>163</v>
-      </c>
-      <c r="D86" s="29">
-        <v>2600</v>
+        <v>16</v>
+      </c>
+      <c r="D86" s="29" t="s">
+        <v>204</v>
       </c>
       <c r="E86" s="29" t="s">
-        <v>34</v>
+        <v>58</v>
       </c>
       <c r="F86" s="29" t="s">
         <v>13</v>
       </c>
       <c r="G86" s="24" t="s">
-        <v>201</v>
+        <v>207</v>
       </c>
       <c r="H86" s="24" t="s">
         <v>203</v>
@@ -3854,13 +3889,13 @@
         <v>2600</v>
       </c>
       <c r="E87" s="29" t="s">
-        <v>58</v>
+        <v>34</v>
       </c>
       <c r="F87" s="29" t="s">
         <v>13</v>
       </c>
       <c r="G87" s="24" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="H87" s="24" t="s">
         <v>203</v>
@@ -3881,13 +3916,13 @@
         <v>2600</v>
       </c>
       <c r="E88" s="29" t="s">
-        <v>58</v>
+        <v>34</v>
       </c>
       <c r="F88" s="29" t="s">
         <v>13</v>
       </c>
       <c r="G88" s="24" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
       <c r="H88" s="24" t="s">
         <v>203</v>
@@ -3908,21 +3943,129 @@
         <v>2600</v>
       </c>
       <c r="E89" s="29" t="s">
-        <v>58</v>
+        <v>34</v>
       </c>
       <c r="F89" s="29" t="s">
         <v>13</v>
       </c>
       <c r="G89" s="24" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="H89" s="24" t="s">
         <v>203</v>
       </c>
       <c r="I89" s="29"/>
     </row>
+    <row r="90" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A90" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="B90" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="C90" s="24" t="s">
+        <v>163</v>
+      </c>
+      <c r="D90" s="29">
+        <v>2600</v>
+      </c>
+      <c r="E90" s="29" t="s">
+        <v>34</v>
+      </c>
+      <c r="F90" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="G90" s="24" t="s">
+        <v>201</v>
+      </c>
+      <c r="H90" s="24" t="s">
+        <v>203</v>
+      </c>
+      <c r="I90" s="29"/>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A91" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="B91" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="C91" s="24" t="s">
+        <v>163</v>
+      </c>
+      <c r="D91" s="29">
+        <v>2600</v>
+      </c>
+      <c r="E91" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="F91" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="G91" s="24" t="s">
+        <v>205</v>
+      </c>
+      <c r="H91" s="24" t="s">
+        <v>203</v>
+      </c>
+      <c r="I91" s="29"/>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A92" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="B92" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="C92" s="24" t="s">
+        <v>163</v>
+      </c>
+      <c r="D92" s="29">
+        <v>2600</v>
+      </c>
+      <c r="E92" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="F92" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="G92" s="24" t="s">
+        <v>206</v>
+      </c>
+      <c r="H92" s="24" t="s">
+        <v>203</v>
+      </c>
+      <c r="I92" s="29"/>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A93" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="B93" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="C93" s="24" t="s">
+        <v>163</v>
+      </c>
+      <c r="D93" s="29">
+        <v>2600</v>
+      </c>
+      <c r="E93" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="F93" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="G93" s="24" t="s">
+        <v>207</v>
+      </c>
+      <c r="H93" s="24" t="s">
+        <v>203</v>
+      </c>
+      <c r="I93" s="29"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:I73" xr:uid="{BE8EF00C-546C-4458-B0BC-6A95E4BA2A0B}"/>
+  <autoFilter ref="A1:I93" xr:uid="{BE8EF00C-546C-4458-B0BC-6A95E4BA2A0B}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>

</xml_diff>

<commit_message>
update path for ericsson 2g
</commit_message>
<xml_diff>
--- a/config/prod/RawFilePathCollection.xlsx
+++ b/config/prod/RawFilePathCollection.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Libraries\git\true\RanBaselineApp\source\config\prod\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB5F8768-B632-474F-A354-58C1369EDF15}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A706F1CC-7FD6-4E6B-A617-592E01761486}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{F32754BE-CF86-49F4-BEFD-53C8D448A04A}"/>
   </bookViews>
@@ -204,7 +204,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1721" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1721" uniqueCount="219">
   <si>
     <t>ZTE</t>
   </si>
@@ -855,6 +855,12 @@
   </si>
   <si>
     <t>/home/app/ngoss/data/rfserver/UtranLTE/NOE/BTS3900_LTE3/1Current/</t>
+  </si>
+  <si>
+    <t>/home/app/ngoss/data/rfserver/Ericsson/CEW-ENM/CNA_FULL/1Current/</t>
+  </si>
+  <si>
+    <t>/home/app/ngoss/data/rfserver/Ericsson/CEW-ENM/EXERT/1Current/</t>
   </si>
 </sst>
 </file>
@@ -1391,7 +1397,7 @@
   <dimension ref="A1:I93"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.19921875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1456,7 +1462,7 @@
         <v>13</v>
       </c>
       <c r="G2" s="24" t="s">
-        <v>81</v>
+        <v>217</v>
       </c>
       <c r="H2" s="24" t="s">
         <v>49</v>
@@ -1485,7 +1491,7 @@
         <v>13</v>
       </c>
       <c r="G3" s="24" t="s">
-        <v>82</v>
+        <v>218</v>
       </c>
       <c r="H3" s="24" t="s">
         <v>60</v>

</xml_diff>

<commit_message>
Add ericsson mixedmode NL
</commit_message>
<xml_diff>
--- a/config/prod/RawFilePathCollection.xlsx
+++ b/config/prod/RawFilePathCollection.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Libraries\git\true\RanBaselineApp\source\config\prod\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A706F1CC-7FD6-4E6B-A617-592E01761486}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF877A57-671F-441B-BF45-C653127BCA8F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{F32754BE-CF86-49F4-BEFD-53C8D448A04A}"/>
   </bookViews>
@@ -204,7 +204,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1721" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1775" uniqueCount="225">
   <si>
     <t>ZTE</t>
   </si>
@@ -861,13 +861,31 @@
   </si>
   <si>
     <t>/home/app/ngoss/data/rfserver/Ericsson/CEW-ENM/EXERT/1Current/</t>
+  </si>
+  <si>
+    <t>/home/app/ngoss/data/rfserver/Ericsson/NTH-ENM/full_kget/MIXEDMODE_NL/1Current</t>
+  </si>
+  <si>
+    <t>/home/app/ngoss/data/rfserver/Ericsson/STH-ENM/full_kget/MIXEDMODE_NL/1Current</t>
+  </si>
+  <si>
+    <t>/home/app/ngoss/data/rfserver/Ericsson/CEW-ENM/full_kget/MIXEDMODE_NL/1Current</t>
+  </si>
+  <si>
+    <t>700/2600</t>
+  </si>
+  <si>
+    <t>700/2601</t>
+  </si>
+  <si>
+    <t>700/2602</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -905,6 +923,12 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1394,10 +1418,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B114B3C2-9B56-4F69-A484-BA4ED1CFE527}">
-  <dimension ref="A1:I93"/>
+  <dimension ref="A1:I99"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" topLeftCell="A73" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G104" sqref="G104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.19921875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -4070,8 +4094,183 @@
       </c>
       <c r="I93" s="29"/>
     </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A94" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="B94" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="C94" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="D94" s="29" t="s">
+        <v>54</v>
+      </c>
+      <c r="E94" s="29" t="s">
+        <v>55</v>
+      </c>
+      <c r="F94" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="G94" s="24" t="s">
+        <v>219</v>
+      </c>
+      <c r="H94" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="I94" s="29" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A95" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="B95" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="C95" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="D95" s="29" t="s">
+        <v>54</v>
+      </c>
+      <c r="E95" s="29" t="s">
+        <v>46</v>
+      </c>
+      <c r="F95" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="G95" s="24" t="s">
+        <v>220</v>
+      </c>
+      <c r="H95" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="I95" s="29" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A96" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="B96" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="C96" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="D96" s="29" t="s">
+        <v>54</v>
+      </c>
+      <c r="E96" s="29" t="s">
+        <v>48</v>
+      </c>
+      <c r="F96" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="G96" s="24" t="s">
+        <v>221</v>
+      </c>
+      <c r="H96" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="I96" s="29" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A97" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="B97" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="C97" s="24" t="s">
+        <v>163</v>
+      </c>
+      <c r="D97" s="29" t="s">
+        <v>222</v>
+      </c>
+      <c r="E97" s="29" t="s">
+        <v>55</v>
+      </c>
+      <c r="F97" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="G97" s="24" t="s">
+        <v>219</v>
+      </c>
+      <c r="H97" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="I97" s="29" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A98" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="B98" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="C98" s="24" t="s">
+        <v>163</v>
+      </c>
+      <c r="D98" s="29" t="s">
+        <v>223</v>
+      </c>
+      <c r="E98" s="29" t="s">
+        <v>46</v>
+      </c>
+      <c r="F98" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="G98" s="24" t="s">
+        <v>220</v>
+      </c>
+      <c r="H98" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="I98" s="29" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A99" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="B99" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="C99" s="24" t="s">
+        <v>163</v>
+      </c>
+      <c r="D99" s="29" t="s">
+        <v>224</v>
+      </c>
+      <c r="E99" s="29" t="s">
+        <v>48</v>
+      </c>
+      <c r="F99" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="G99" s="24" t="s">
+        <v>221</v>
+      </c>
+      <c r="H99" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="I99" s="29" t="s">
+        <v>52</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:I93" xr:uid="{BE8EF00C-546C-4458-B0BC-6A95E4BA2A0B}"/>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>

</xml_diff>

<commit_message>
Update path ENM1 for 2G
</commit_message>
<xml_diff>
--- a/config/prod/RawFilePathCollection.xlsx
+++ b/config/prod/RawFilePathCollection.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Libraries\git\true\RanBaselineApp\source\config\prod\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF877A57-671F-441B-BF45-C653127BCA8F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76919503-FDB0-4976-99B1-EA51B215597C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{F32754BE-CF86-49F4-BEFD-53C8D448A04A}"/>
   </bookViews>
@@ -204,7 +204,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1775" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1775" uniqueCount="227">
   <si>
     <t>ZTE</t>
   </si>
@@ -879,6 +879,12 @@
   </si>
   <si>
     <t>700/2602</t>
+  </si>
+  <si>
+    <t>/home/app/ngoss/data/rfserver/Ericsson/NTH-ENM/CNA_FULL/1Current/</t>
+  </si>
+  <si>
+    <t>/home/app/ngoss/data/rfserver/Ericsson/NTH-ENM/EXERT/1Current/</t>
   </si>
 </sst>
 </file>
@@ -1420,8 +1426,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B114B3C2-9B56-4F69-A484-BA4ED1CFE527}">
   <dimension ref="A1:I99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G104" sqref="G104"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.19921875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1544,7 +1550,7 @@
         <v>13</v>
       </c>
       <c r="G4" s="24" t="s">
-        <v>83</v>
+        <v>225</v>
       </c>
       <c r="H4" s="24" t="s">
         <v>49</v>
@@ -1573,7 +1579,7 @@
         <v>13</v>
       </c>
       <c r="G5" s="24" t="s">
-        <v>84</v>
+        <v>226</v>
       </c>
       <c r="H5" s="24" t="s">
         <v>56</v>

</xml_diff>